<commit_message>
other stuff for survey
</commit_message>
<xml_diff>
--- a/survey1/News recommender_October 14, 2023_12.50.xlsx
+++ b/survey1/News recommender_October 14, 2023_12.50.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangf\Myrepos\MINDFUL-A-Lenskit-based-Recommender-System\survey1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcroe\PycharmProjects\MINDFUL-A-Lenskit-based-Recommender-System\survey1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61B12E5-FD2C-4394-A423-89C17DAD6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2057A90A-CEF8-4974-BB44-9598D291DA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="432" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$3:$BA$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$4:$BA$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="233">
   <si>
     <t>StartDate</t>
   </si>
@@ -696,6 +696,126 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>Job scam promising $26 an hour starts with Goo...</t>
+  </si>
+  <si>
+    <t>Are you in a relationship with a coworker? Rea...</t>
+  </si>
+  <si>
+    <t>50 Great Jobs for Retirees</t>
+  </si>
+  <si>
+    <t>Walmart employees reveal how much they really ...</t>
+  </si>
+  <si>
+    <t>Now That I'm Over 50, I'm Finally Sucking It U...</t>
+  </si>
+  <si>
+    <t>Science Says Doing This One Thing for 15 Minut...</t>
+  </si>
+  <si>
+    <t>Bank of America declares the end of the 60-40 ...</t>
+  </si>
+  <si>
+    <t>The 25 best mutual funds of all time</t>
+  </si>
+  <si>
+    <t>2020 Ford Mustang Shelby GT500: First Drive Re...</t>
+  </si>
+  <si>
+    <t>Lamborghini Urus vs. Dodge Challenger Hellcat ...</t>
+  </si>
+  <si>
+    <t>5 reasons Gen Xers are struggling with retirem...</t>
+  </si>
+  <si>
+    <t>What to do if your employer changes the terms ...</t>
+  </si>
+  <si>
+    <t>Sounders vs. Real Salt Lake, talking points: L...</t>
+  </si>
+  <si>
+    <t>Winners &amp; Losers: Sounders 4, FC Dallas 3</t>
+  </si>
+  <si>
+    <t>Sausages Sold At Walmart Recalled For Possible...</t>
+  </si>
+  <si>
+    <t>Her cancer surgery was a success. Then a genet...</t>
+  </si>
+  <si>
+    <t>'Bachelor's Amanda Stanton Is Dating 'Rich Kid...</t>
+  </si>
+  <si>
+    <t>Kelly Ripa responds to backlash over son in 'e...</t>
+  </si>
+  <si>
+    <t>The Cost of Trump's Aid Freeze in the Trenches...</t>
+  </si>
+  <si>
+    <t>Chile: Three die in supermarket fire amid prot...</t>
+  </si>
+  <si>
+    <t>Diahann Carroll, Pioneering Actress on 'Julia'...</t>
+  </si>
+  <si>
+    <t>Octavia Spencer Delivers Rousing Speech About ...</t>
+  </si>
+  <si>
+    <t>Denver Broncos quarterback Joe Flacco voices f...</t>
+  </si>
+  <si>
+    <t>Can't-Miss Play: Marquez Valdes-Scantling torc...</t>
+  </si>
+  <si>
+    <t>'El Camino: A Breaking Bad Movie': TV Review</t>
+  </si>
+  <si>
+    <t>'The Little Mermaid Live!': TV Review</t>
+  </si>
+  <si>
+    <t>Michigan finally shows some fight, but can't s...</t>
+  </si>
+  <si>
+    <t>Locked On Suns Wednesday: Suns blast Kings to ...</t>
+  </si>
+  <si>
+    <t>Touch and go: The trouble (and danger) with to...</t>
+  </si>
+  <si>
+    <t>Ford owners love this little-known feature oth...</t>
+  </si>
+  <si>
+    <t>Woman loses her mother's wedding ring while pa...</t>
+  </si>
+  <si>
+    <t>How Avoid a Sexless Marriage: 9 Tips From Happ...</t>
+  </si>
+  <si>
+    <t>Where to Find a Good, Cheap Sandwich in Every ...</t>
+  </si>
+  <si>
+    <t>16 major chains where you can buy plant-based ...</t>
+  </si>
+  <si>
+    <t>America's Biggest Trash Hauler Stops Shipping ...</t>
+  </si>
+  <si>
+    <t>The size of a bus, rare and endangered whale s...</t>
+  </si>
+  <si>
+    <t>2019 Tokyo Motor Show in Photos: A Visual Tour</t>
+  </si>
+  <si>
+    <t>Toyota LQ self-driving concept car is at your ...</t>
+  </si>
+  <si>
+    <t>The Brands Queen Elizabeth, Prince Charles, an...</t>
+  </si>
+  <si>
+    <t>Kate Middleton's Best Hairstyles Through the Y...</t>
   </si>
 </sst>
 </file>
@@ -769,7 +889,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -796,7 +916,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1092,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA42"/>
+  <dimension ref="A1:BA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT30" sqref="AT30"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,299 +1226,262 @@
     <col min="12" max="12" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N1" s="6" t="s">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1" t="s">
+        <v>198</v>
+      </c>
+      <c r="T1" t="s">
+        <v>199</v>
+      </c>
+      <c r="U1" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" t="s">
+        <v>201</v>
+      </c>
+      <c r="W1" t="s">
+        <v>202</v>
+      </c>
+      <c r="X1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>231</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
@@ -1410,309 +1493,307 @@
         <v>6</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AN3" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AV3" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AX3" s="3" t="s">
+      <c r="AX4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="AY4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="AZ4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BA4" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="5" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>45212.652291666665</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>45212.654745370368</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>212</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="1">
-        <v>45212.654759895835</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AQ4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AT4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BA4" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>45212.673495370371</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45212.677800925929</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>55</v>
@@ -1724,16 +1805,16 @@
         <v>100</v>
       </c>
       <c r="F5">
-        <v>371</v>
+        <v>212</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H5" s="1">
-        <v>45212.677819571756</v>
+        <v>45212.654759895835</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>104</v>
@@ -1742,40 +1823,40 @@
         <v>105</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>107</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>107</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>108</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>108</v>
@@ -1793,16 +1874,16 @@
         <v>107</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD5" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>107</v>
@@ -1823,13 +1904,13 @@
         <v>108</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AN5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AP5" s="2" t="s">
         <v>107</v>
@@ -1838,22 +1919,22 @@
         <v>107</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS5" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AT5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AV5" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AW5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AX5" s="2" t="s">
         <v>107</v>
@@ -1862,18 +1943,18 @@
         <v>107</v>
       </c>
       <c r="AZ5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BA5" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45212.674537037034</v>
+        <v>45212.673495370371</v>
       </c>
       <c r="B6" s="1">
-        <v>45212.686168981483</v>
+        <v>45212.677800925929</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>55</v>
@@ -1885,16 +1966,16 @@
         <v>100</v>
       </c>
       <c r="F6">
-        <v>1005</v>
+        <v>371</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H6" s="1">
-        <v>45212.686184618055</v>
+        <v>45212.677819571756</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>104</v>
@@ -1903,34 +1984,34 @@
         <v>105</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>108</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T6" s="2" t="s">
         <v>108</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>108</v>
@@ -1954,16 +2035,16 @@
         <v>107</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AD6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>107</v>
@@ -1981,16 +2062,16 @@
         <v>107</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AN6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AP6" s="2" t="s">
         <v>107</v>
@@ -1999,7 +2080,7 @@
         <v>107</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AS6" s="2" t="s">
         <v>108</v>
@@ -2008,13 +2089,13 @@
         <v>108</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AV6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AW6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AX6" s="2" t="s">
         <v>107</v>
@@ -2023,18 +2104,18 @@
         <v>107</v>
       </c>
       <c r="AZ6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BA6" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45213.173611111109</v>
+        <v>45212.674537037034</v>
       </c>
       <c r="B7" s="1">
-        <v>45213.178530092591</v>
+        <v>45212.686168981483</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
@@ -2046,16 +2127,16 @@
         <v>100</v>
       </c>
       <c r="F7">
-        <v>424</v>
+        <v>1005</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H7" s="1">
-        <v>45213.178541597219</v>
+        <v>45212.686184618055</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>104</v>
@@ -2064,13 +2145,13 @@
         <v>105</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>108</v>
@@ -2082,10 +2163,10 @@
         <v>108</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>108</v>
@@ -2109,25 +2190,25 @@
         <v>107</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH7" s="2" t="s">
         <v>107</v>
@@ -2136,7 +2217,7 @@
         <v>107</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>107</v>
@@ -2148,16 +2229,16 @@
         <v>107</v>
       </c>
       <c r="AN7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AO7" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR7" s="2" t="s">
         <v>107</v>
@@ -2169,10 +2250,10 @@
         <v>108</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AW7" s="2" t="s">
         <v>107</v>
@@ -2181,21 +2262,21 @@
         <v>107</v>
       </c>
       <c r="AY7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AZ7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BA7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45213.214074074072</v>
+        <v>45213.173611111109</v>
       </c>
       <c r="B8" s="1">
-        <v>45213.215462962966</v>
+        <v>45213.178530092591</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>55</v>
@@ -2207,16 +2288,16 @@
         <v>100</v>
       </c>
       <c r="F8">
-        <v>119</v>
+        <v>424</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H8" s="1">
-        <v>45213.21547466435</v>
+        <v>45213.178541597219</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>104</v>
@@ -2225,22 +2306,22 @@
         <v>105</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>107</v>
@@ -2249,7 +2330,7 @@
         <v>107</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>108</v>
@@ -2258,13 +2339,13 @@
         <v>108</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>108</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>107</v>
@@ -2279,19 +2360,19 @@
         <v>108</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI8" s="2" t="s">
         <v>107</v>
@@ -2303,7 +2384,7 @@
         <v>107</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AM8" s="2" t="s">
         <v>107</v>
@@ -2324,7 +2405,7 @@
         <v>107</v>
       </c>
       <c r="AS8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AT8" s="2" t="s">
         <v>108</v>
@@ -2333,13 +2414,13 @@
         <v>108</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AW8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AX8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AY8" s="2" t="s">
         <v>108</v>
@@ -2348,15 +2429,15 @@
         <v>108</v>
       </c>
       <c r="BA8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45213.21234953704</v>
+        <v>45213.214074074072</v>
       </c>
       <c r="B9" s="1">
-        <v>45213.215682870374</v>
+        <v>45213.215462962966</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>55</v>
@@ -2368,16 +2449,16 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>288</v>
+        <v>119</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H9" s="1">
-        <v>45213.215699687498</v>
+        <v>45213.21547466435</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>104</v>
@@ -2386,22 +2467,22 @@
         <v>105</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>107</v>
@@ -2422,7 +2503,7 @@
         <v>107</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>107</v>
@@ -2431,28 +2512,28 @@
         <v>107</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AE9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AI9" s="2" t="s">
         <v>107</v>
@@ -2461,63 +2542,63 @@
         <v>108</v>
       </c>
       <c r="AK9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AN9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AO9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AP9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AQ9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AT9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AV9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AW9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AX9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AY9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AZ9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BA9" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:53" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45213.357685185183</v>
+        <v>45213.21234953704</v>
       </c>
       <c r="B10" s="1">
-        <v>45213.361203703702</v>
+        <v>45213.215682870374</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>55</v>
@@ -2529,16 +2610,16 @@
         <v>100</v>
       </c>
       <c r="F10">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H10" s="1">
-        <v>45213.361223171298</v>
+        <v>45213.215699687498</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>104</v>
@@ -2547,16 +2628,16 @@
         <v>105</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>108</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>107</v>
@@ -2577,7 +2658,7 @@
         <v>108</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>107</v>
@@ -2595,10 +2676,10 @@
         <v>107</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AD10" s="2" t="s">
         <v>108</v>
@@ -2610,7 +2691,7 @@
         <v>107</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AH10" s="2" t="s">
         <v>107</v>
@@ -2619,16 +2700,16 @@
         <v>107</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AN10" s="2" t="s">
         <v>107</v>
@@ -2640,13 +2721,13 @@
         <v>107</v>
       </c>
       <c r="AQ10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AS10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AT10" s="2" t="s">
         <v>108</v>
@@ -2658,13 +2739,13 @@
         <v>107</v>
       </c>
       <c r="AW10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AX10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AY10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AZ10" s="2" t="s">
         <v>107</v>
@@ -2673,12 +2754,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45213.358599537038</v>
+        <v>45213.357685185183</v>
       </c>
       <c r="B11" s="1">
-        <v>45213.362407407411</v>
+        <v>45213.361203703702</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>55</v>
@@ -2690,16 +2771,16 @@
         <v>100</v>
       </c>
       <c r="F11">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H11" s="1">
-        <v>45213.362416261574</v>
+        <v>45213.361223171298</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>104</v>
@@ -2708,16 +2789,16 @@
         <v>105</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>108</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>107</v>
@@ -2729,10 +2810,10 @@
         <v>107</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>108</v>
@@ -2744,7 +2825,7 @@
         <v>107</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y11" s="2" t="s">
         <v>107</v>
@@ -2756,13 +2837,13 @@
         <v>107</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC11" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AE11" s="2" t="s">
         <v>107</v>
@@ -2771,7 +2852,7 @@
         <v>107</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH11" s="2" t="s">
         <v>107</v>
@@ -2798,7 +2879,7 @@
         <v>107</v>
       </c>
       <c r="AP11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ11" s="2" t="s">
         <v>107</v>
@@ -2807,7 +2888,7 @@
         <v>107</v>
       </c>
       <c r="AS11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AT11" s="2" t="s">
         <v>108</v>
@@ -2819,10 +2900,10 @@
         <v>107</v>
       </c>
       <c r="AW11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AX11" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AY11" s="2" t="s">
         <v>108</v>
@@ -2836,10 +2917,10 @@
     </row>
     <row r="12" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45213.361388888887</v>
+        <v>45213.358599537038</v>
       </c>
       <c r="B12" s="1">
-        <v>45213.364571759259</v>
+        <v>45213.362407407411</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>55</v>
@@ -2851,16 +2932,16 @@
         <v>100</v>
       </c>
       <c r="F12">
-        <v>275</v>
+        <v>328</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H12" s="1">
-        <v>45213.364590821759</v>
+        <v>45213.362416261574</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>104</v>
@@ -2869,28 +2950,28 @@
         <v>105</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>108</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>107</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T12" s="2" t="s">
         <v>108</v>
@@ -2899,16 +2980,16 @@
         <v>108</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>108</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Z12" s="2" t="s">
         <v>107</v>
@@ -2917,10 +2998,10 @@
         <v>107</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD12" s="2" t="s">
         <v>107</v>
@@ -2929,7 +3010,7 @@
         <v>107</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>108</v>
@@ -2938,7 +3019,7 @@
         <v>107</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ12" s="2" t="s">
         <v>107</v>
@@ -2947,7 +3028,7 @@
         <v>107</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AM12" s="2" t="s">
         <v>107</v>
@@ -2962,25 +3043,25 @@
         <v>108</v>
       </c>
       <c r="AQ12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AT12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AU12" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AW12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AX12" s="2" t="s">
         <v>107</v>
@@ -2997,10 +3078,10 @@
     </row>
     <row r="13" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45213.361655092594</v>
+        <v>45213.361388888887</v>
       </c>
       <c r="B13" s="1">
-        <v>45213.365023148152</v>
+        <v>45213.364571759259</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>55</v>
@@ -3012,16 +3093,16 @@
         <v>100</v>
       </c>
       <c r="F13">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H13" s="1">
-        <v>45213.365038043979</v>
+        <v>45213.364590821759</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>104</v>
@@ -3030,46 +3111,46 @@
         <v>105</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>107</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Z13" s="2" t="s">
         <v>107</v>
@@ -3078,10 +3159,10 @@
         <v>107</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AD13" s="2" t="s">
         <v>107</v>
@@ -3093,7 +3174,7 @@
         <v>108</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AH13" s="2" t="s">
         <v>107</v>
@@ -3111,7 +3192,7 @@
         <v>107</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AN13" s="2" t="s">
         <v>107</v>
@@ -3120,10 +3201,10 @@
         <v>107</v>
       </c>
       <c r="AP13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AQ13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AR13" s="2" t="s">
         <v>108</v>
@@ -3132,7 +3213,7 @@
         <v>107</v>
       </c>
       <c r="AT13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AU13" s="2" t="s">
         <v>107</v>
@@ -3147,21 +3228,21 @@
         <v>107</v>
       </c>
       <c r="AY13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AZ13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BA13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:53" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45213.366180555553</v>
+        <v>45213.361655092594</v>
       </c>
       <c r="B14" s="1">
-        <v>45213.36922453704</v>
+        <v>45213.365023148152</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>55</v>
@@ -3173,16 +3254,16 @@
         <v>100</v>
       </c>
       <c r="F14">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H14" s="1">
-        <v>45213.369236331018</v>
+        <v>45213.365038043979</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>104</v>
@@ -3191,10 +3272,10 @@
         <v>105</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>107</v>
@@ -3203,7 +3284,7 @@
         <v>108</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>108</v>
@@ -3218,13 +3299,13 @@
         <v>107</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>107</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>107</v>
@@ -3251,7 +3332,7 @@
         <v>107</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG14" s="2" t="s">
         <v>107</v>
@@ -3260,7 +3341,7 @@
         <v>107</v>
       </c>
       <c r="AI14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AJ14" s="2" t="s">
         <v>107</v>
@@ -3272,7 +3353,7 @@
         <v>107</v>
       </c>
       <c r="AM14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AN14" s="2" t="s">
         <v>107</v>
@@ -3284,10 +3365,10 @@
         <v>107</v>
       </c>
       <c r="AQ14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AS14" s="2" t="s">
         <v>107</v>
@@ -3302,7 +3383,7 @@
         <v>108</v>
       </c>
       <c r="AW14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AX14" s="2" t="s">
         <v>107</v>
@@ -3311,18 +3392,18 @@
         <v>107</v>
       </c>
       <c r="AZ14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BA14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45213.37159722222</v>
+        <v>45213.366180555553</v>
       </c>
       <c r="B15" s="1">
-        <v>45213.378263888888</v>
+        <v>45213.36922453704</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>55</v>
@@ -3334,16 +3415,16 @@
         <v>100</v>
       </c>
       <c r="F15">
-        <v>576</v>
+        <v>262</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H15" s="1">
-        <v>45213.378280185185</v>
+        <v>45213.369236331018</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>104</v>
@@ -3352,22 +3433,22 @@
         <v>105</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>107</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>108</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>107</v>
@@ -3379,10 +3460,10 @@
         <v>107</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W15" s="2" t="s">
         <v>108</v>
@@ -3397,7 +3478,7 @@
         <v>107</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AB15" s="2" t="s">
         <v>107</v>
@@ -3421,28 +3502,28 @@
         <v>107</v>
       </c>
       <c r="AI15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ15" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AK15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AN15" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AO15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AP15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ15" s="2" t="s">
         <v>108</v>
@@ -3457,7 +3538,7 @@
         <v>108</v>
       </c>
       <c r="AU15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AV15" s="2" t="s">
         <v>108</v>
@@ -3466,10 +3547,10 @@
         <v>108</v>
       </c>
       <c r="AX15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AY15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AZ15" s="2" t="s">
         <v>107</v>
@@ -3480,10 +3561,10 @@
     </row>
     <row r="16" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45213.435868055552</v>
+        <v>45213.37159722222</v>
       </c>
       <c r="B16" s="1">
-        <v>45213.463402777779</v>
+        <v>45213.378263888888</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>55</v>
@@ -3495,16 +3576,16 @@
         <v>100</v>
       </c>
       <c r="F16">
-        <v>2379</v>
+        <v>576</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H16" s="1">
-        <v>45213.463423275462</v>
+        <v>45213.378280185185</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>104</v>
@@ -3513,10 +3594,10 @@
         <v>105</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>107</v>
@@ -3525,28 +3606,28 @@
         <v>107</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>107</v>
@@ -3558,13 +3639,13 @@
         <v>107</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD16" s="2" t="s">
         <v>107</v>
@@ -3582,25 +3663,25 @@
         <v>107</v>
       </c>
       <c r="AI16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AJ16" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AK16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AN16" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AO16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AP16" s="2" t="s">
         <v>108</v>
@@ -3615,22 +3696,22 @@
         <v>107</v>
       </c>
       <c r="AT16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AU16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AV16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AW16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AX16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AY16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AZ16" s="2" t="s">
         <v>107</v>
@@ -3641,10 +3722,10 @@
     </row>
     <row r="17" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45213.503842592596</v>
+        <v>45213.435868055552</v>
       </c>
       <c r="B17" s="1">
-        <v>45213.514108796298</v>
+        <v>45213.463402777779</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>55</v>
@@ -3656,16 +3737,16 @@
         <v>100</v>
       </c>
       <c r="F17">
-        <v>887</v>
+        <v>2379</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H17" s="1">
-        <v>45213.51412378472</v>
+        <v>45213.463423275462</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>104</v>
@@ -3674,25 +3755,25 @@
         <v>105</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>107</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>107</v>
@@ -3701,10 +3782,10 @@
         <v>108</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W17" s="2" t="s">
         <v>107</v>
@@ -3737,13 +3818,13 @@
         <v>107</v>
       </c>
       <c r="AG17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH17" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AI17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ17" s="2" t="s">
         <v>107</v>
@@ -3755,7 +3836,7 @@
         <v>107</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AN17" s="2" t="s">
         <v>107</v>
@@ -3767,25 +3848,25 @@
         <v>108</v>
       </c>
       <c r="AQ17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AR17" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AS17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AT17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AU17" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AV17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AW17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AX17" s="2" t="s">
         <v>107</v>
@@ -3802,10 +3883,10 @@
     </row>
     <row r="18" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>45213.509502314817</v>
+        <v>45213.503842592596</v>
       </c>
       <c r="B18" s="1">
-        <v>45213.514687499999</v>
+        <v>45213.514108796298</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>55</v>
@@ -3817,16 +3898,16 @@
         <v>100</v>
       </c>
       <c r="F18">
-        <v>448</v>
+        <v>887</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H18" s="1">
-        <v>45213.514705995367</v>
+        <v>45213.51412378472</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>104</v>
@@ -3835,153 +3916,299 @@
         <v>105</v>
       </c>
       <c r="L18" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA18" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45213.509502314817</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45213.514687499999</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>448</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="1">
+        <v>45213.514705995367</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AQ18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AS18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AU18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BA18" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
+      <c r="N19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA19" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
@@ -3993,31 +4220,23 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="AH26" s="7"/>
-      <c r="AI26" s="7"/>
-      <c r="AJ26" s="7"/>
-      <c r="AK26" s="7"/>
-      <c r="AL26" s="7"/>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
@@ -4027,8 +4246,20 @@
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="7"/>
+      <c r="AL27" s="7"/>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
@@ -4038,17 +4269,11 @@
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="6"/>
-      <c r="AG28" s="6"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
@@ -4064,39 +4289,45 @@
       <c r="AE29" s="6"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
-      <c r="AH29" s="6"/>
-      <c r="AI29" s="6"/>
-      <c r="AJ29" s="6"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="P30" t="s">
-        <v>192</v>
-      </c>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AH30" s="6"/>
+      <c r="AI30" s="6"/>
       <c r="AJ30" s="6"/>
-      <c r="AK30" s="6"/>
-      <c r="AL30" s="6"/>
-      <c r="AM30" s="6"/>
-      <c r="AN30" s="6"/>
-      <c r="AO30" s="6"/>
-      <c r="AP30" s="6"/>
-      <c r="AQ30" s="6"/>
-      <c r="AR30" s="6"/>
-      <c r="AS30" s="6"/>
-      <c r="AT30" s="6"/>
-      <c r="AU30" s="6"/>
-      <c r="AV30" s="6"/>
-      <c r="AW30" s="6"/>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
+      <c r="P31" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ31" s="6"/>
+      <c r="AK31" s="6"/>
+      <c r="AL31" s="6"/>
+      <c r="AM31" s="6"/>
+      <c r="AN31" s="6"/>
+      <c r="AO31" s="6"/>
+      <c r="AP31" s="6"/>
+      <c r="AQ31" s="6"/>
+      <c r="AR31" s="6"/>
+      <c r="AS31" s="6"/>
+      <c r="AT31" s="6"/>
+      <c r="AU31" s="6"/>
+      <c r="AV31" s="6"/>
+      <c r="AW31" s="6"/>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.3">
       <c r="P32" s="6"/>
@@ -4119,42 +4350,53 @@
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
     </row>
     <row r="34" spans="12:42" x14ac:dyDescent="0.3">
-      <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
-      <c r="AL34" s="6"/>
-      <c r="AM34" s="6"/>
-      <c r="AN34" s="6"/>
-      <c r="AO34" s="6"/>
-      <c r="AP34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
     </row>
-    <row r="38" spans="12:42" x14ac:dyDescent="0.3">
-      <c r="L38"/>
+    <row r="35" spans="12:42" x14ac:dyDescent="0.3">
+      <c r="AI35" s="6"/>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="6"/>
+      <c r="AL35" s="6"/>
+      <c r="AM35" s="6"/>
+      <c r="AN35" s="6"/>
+      <c r="AO35" s="6"/>
+      <c r="AP35" s="6"/>
     </row>
-    <row r="42" spans="12:42" x14ac:dyDescent="0.3">
-      <c r="AJ42" s="6"/>
-      <c r="AK42" s="6"/>
-      <c r="AL42" s="6"/>
-      <c r="AM42" s="6"/>
-      <c r="AN42" s="6"/>
+    <row r="39" spans="12:42" x14ac:dyDescent="0.3">
+      <c r="L39"/>
+    </row>
+    <row r="43" spans="12:42" x14ac:dyDescent="0.3">
+      <c r="AJ43" s="6"/>
+      <c r="AK43" s="6"/>
+      <c r="AL43" s="6"/>
+      <c r="AM43" s="6"/>
+      <c r="AN43" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:BA19" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="N4:BA18">
+  <autoFilter ref="A4:BA20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N5:BA19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C18 D2:D18 G2:G18 I2:I18 J2:J18 K2:K18 M2:M18 N2:N18 O2:O14 P2:P18 Q2:Q18 R2:R18 S2:S18 T2:T18 U2:U18 V2:V18 W2:W18 X2:X18 Y2:Y18 Z2:Z18 AA2:AA18 AB2:AB18 AC2:AC18 AD2:AD18 AE2:AE18 AF2:AF18 AG2:AG18 AH2:AH18 AI2:AI18 AJ2:AJ18 AK2:AK18 AL2:AL18 AM2:AM18 AN2:AN14 AO2:AO18 AP2:AP18 AQ2:AQ18 AR2:AR18 AS2:AS18 AT2:AT18 AU2:AU18 AV2:AV18 AW2:AW18 AX2:AX18 AY2:AY18 AZ2:AZ18 BA2:BA18 O16:O18 AN16:AN18" numberStoredAsText="1"/>
+    <ignoredError sqref="C3:C19 D3:D19 G3:G19 I3:I19 J3:J19 K3:K19 M3:M19 N3:N19 O3:O15 P3:P19 Q3:Q19 R3:R19 S3:S19 T3:T19 U3:U19 V3:V19 W3:W19 X3:X19 Y3:Y19 Z3:Z19 AA3:AA19 AB3:AB19 AC3:AC19 AD3:AD19 AE3:AE19 AF3:AF19 AG3:AG19 AH3:AH19 AI3:AI19 AJ3:AJ19 AK3:AK19 AL3:AL19 AM3:AM19 AN3:AN15 AO3:AO19 AP3:AP19 AQ3:AQ19 AR3:AR19 AS3:AS19 AT3:AT19 AU3:AU19 AV3:AV19 AW3:AW19 AX3:AX19 AY3:AY19 AZ3:AZ19 BA3:BA19 O17:O19 AN17:AN19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>